<commit_message>
Update BW1099DS & IO Table
</commit_message>
<xml_diff>
--- a/SoMs/BW1099/BW1099_IO_TABLE.xlsx
+++ b/SoMs/BW1099/BW1099_IO_TABLE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BrianLuxonis\Documents\GitHub\depthai-hardware\SoMs\BW1099\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BrianLuxonis\Desktop\hardware\Luxonis_HW_Documentation\BW1099 Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E4114D-80F9-45DA-A998-A895C28E0E47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B177EBB-F78F-435D-B03A-0E59207A5B35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{2A677646-14BE-4F73-937F-BE4037A1016C}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$J$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$J$102</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="193">
   <si>
     <t>Pin #</t>
   </si>
@@ -204,9 +204,6 @@
     <t>sd_hst0_dat_3</t>
   </si>
   <si>
-    <t>spi2_ss_0</t>
-  </si>
-  <si>
     <t>pwm_3</t>
   </si>
   <si>
@@ -261,9 +258,6 @@
     <t>1.8V Output</t>
   </si>
   <si>
-    <t>Open-drain output from SoM PMIC indicating SoM. PGOOD=1, PBAD=0.</t>
-  </si>
-  <si>
     <t>sd_hst0_dat_1</t>
   </si>
   <si>
@@ -279,9 +273,6 @@
     <t>1.8V Input</t>
   </si>
   <si>
-    <t>SoM system reset</t>
-  </si>
-  <si>
     <t>sd_hst0_dat_0</t>
   </si>
   <si>
@@ -300,9 +291,6 @@
     <t>PD: 10kR/GND</t>
   </si>
   <si>
-    <t>Used to wake MA2484 from sleep state</t>
-  </si>
-  <si>
     <t>COM_AUX_IO2</t>
   </si>
   <si>
@@ -610,6 +598,24 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open-drain output from SoM PMIC indicating SoM. PGOOD=1, PBAD=0. Leave floating if unused. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SoM system reset. Leave floating if unused. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leave floating.  Any SGPIO pin can be used to wake up the SoM. </t>
+  </si>
+  <si>
+    <t>spi2_cs_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typically labeled as UART_TX on Luxonis baseboards. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typically labeled as UART_RX on Luxonis baseboards. </t>
   </si>
 </sst>
 </file>
@@ -996,7 +1002,7 @@
   <dimension ref="A1:J103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1012,7 +1018,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1032,7 +1038,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
@@ -1053,7 +1059,7 @@
         <v>7</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -1097,10 +1103,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -1110,6 +1116,9 @@
       </c>
       <c r="I6" t="s">
         <v>15</v>
+      </c>
+      <c r="J6" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -1131,10 +1140,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
@@ -1144,6 +1153,9 @@
       </c>
       <c r="I8" t="s">
         <v>15</v>
+      </c>
+      <c r="J8" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1424,7 +1436,7 @@
         <v>49</v>
       </c>
       <c r="C30" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H30" t="s">
         <v>50</v>
@@ -1477,31 +1489,31 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C34" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D34" t="s">
         <v>54</v>
       </c>
       <c r="E34" t="s">
+        <v>190</v>
+      </c>
+      <c r="F34" t="s">
         <v>55</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>56</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>57</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>58</v>
       </c>
-      <c r="I34" t="s">
-        <v>59</v>
-      </c>
       <c r="J34" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
@@ -1509,22 +1521,22 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D35" t="s">
         <v>60</v>
       </c>
-      <c r="C35" t="s">
-        <v>145</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="H35" t="s">
         <v>61</v>
-      </c>
-      <c r="H35" t="s">
-        <v>62</v>
       </c>
       <c r="I35" t="s">
         <v>15</v>
       </c>
       <c r="J35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
@@ -1532,16 +1544,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C36" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="I36" t="s">
         <v>15</v>
       </c>
       <c r="J36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
@@ -1549,19 +1561,19 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I37" t="s">
         <v>15</v>
       </c>
       <c r="J37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
@@ -1569,25 +1581,25 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C38" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D38" t="s">
+        <v>67</v>
+      </c>
+      <c r="E38" t="s">
         <v>68</v>
       </c>
-      <c r="E38" t="s">
+      <c r="H38" t="s">
         <v>69</v>
       </c>
-      <c r="H38" t="s">
-        <v>70</v>
-      </c>
       <c r="I38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J38" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
@@ -1595,16 +1607,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
+        <v>70</v>
+      </c>
+      <c r="H39" t="s">
         <v>71</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>72</v>
       </c>
-      <c r="I39" t="s">
-        <v>73</v>
-      </c>
       <c r="J39" t="s">
-        <v>74</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
@@ -1612,28 +1624,28 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C40" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D40" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" t="s">
+        <v>74</v>
+      </c>
+      <c r="G40" t="s">
         <v>75</v>
       </c>
-      <c r="E40" t="s">
-        <v>76</v>
-      </c>
-      <c r="G40" t="s">
-        <v>77</v>
-      </c>
       <c r="H40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J40" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
@@ -1641,16 +1653,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I41" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J41" t="s">
-        <v>80</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
@@ -1658,31 +1670,31 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D42" t="s">
+        <v>78</v>
+      </c>
+      <c r="E42" t="s">
+        <v>79</v>
+      </c>
+      <c r="F42" t="s">
+        <v>80</v>
+      </c>
+      <c r="G42" t="s">
         <v>81</v>
       </c>
-      <c r="E42" t="s">
-        <v>82</v>
-      </c>
-      <c r="F42" t="s">
-        <v>83</v>
-      </c>
-      <c r="G42" t="s">
-        <v>84</v>
-      </c>
       <c r="H42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J42" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
@@ -1690,16 +1702,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H43" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I43" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J43" t="s">
-        <v>87</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
@@ -1707,16 +1719,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C44" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I44" t="s">
         <v>15</v>
       </c>
       <c r="J44" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
@@ -1768,13 +1780,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I49" t="s">
         <v>9</v>
       </c>
       <c r="J49" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
@@ -1782,13 +1794,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I50" t="s">
         <v>9</v>
       </c>
       <c r="J50" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
@@ -1796,13 +1808,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I51" t="s">
         <v>9</v>
       </c>
       <c r="J51" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
@@ -1810,13 +1822,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I52" t="s">
         <v>9</v>
       </c>
       <c r="J52" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
@@ -1824,13 +1836,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I53" t="s">
         <v>9</v>
       </c>
       <c r="J53" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.35">
@@ -1838,13 +1850,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I54" t="s">
         <v>9</v>
       </c>
       <c r="J54" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
@@ -1852,13 +1864,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I55" t="s">
         <v>9</v>
       </c>
       <c r="J55" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
@@ -1866,13 +1878,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I56" t="s">
         <v>9</v>
       </c>
       <c r="J56" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.35">
@@ -1924,19 +1936,19 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C61" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I61" t="s">
         <v>15</v>
       </c>
       <c r="J61" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
@@ -1944,19 +1956,19 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C62" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D62" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I62" t="s">
         <v>15</v>
       </c>
       <c r="J62" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.35">
@@ -1964,25 +1976,25 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C63" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D63" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E63" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J63" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.35">
@@ -1990,16 +2002,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C64" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="I64" t="s">
         <v>15</v>
       </c>
       <c r="J64" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.35">
@@ -2007,28 +2019,28 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C65" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D65" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E65" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G65" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I65" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J65" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.35">
@@ -2036,16 +2048,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C66" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="I66" t="s">
         <v>15</v>
       </c>
       <c r="J66" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
@@ -2053,16 +2065,16 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C67" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I67" t="s">
         <v>15</v>
       </c>
       <c r="J67" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
@@ -2070,19 +2082,19 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C68" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H68" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I68" t="s">
         <v>15</v>
       </c>
       <c r="J68" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.35">
@@ -2090,16 +2102,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C69" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I69" t="s">
         <v>15</v>
       </c>
       <c r="J69" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.35">
@@ -2107,19 +2119,19 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C70" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H70" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I70" t="s">
         <v>15</v>
       </c>
       <c r="J70" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
@@ -2127,10 +2139,10 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C71" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I71" t="s">
         <v>15</v>
@@ -2141,19 +2153,19 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C72" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H72" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I72" t="s">
         <v>15</v>
       </c>
       <c r="J72" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.35">
@@ -2183,10 +2195,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C75" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H75" t="s">
         <v>50</v>
@@ -2195,7 +2207,7 @@
         <v>15</v>
       </c>
       <c r="J75" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
@@ -2203,16 +2215,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C76" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I76" t="s">
         <v>15</v>
       </c>
       <c r="J76" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
@@ -2242,19 +2254,19 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C79" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="H79" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I79" t="s">
         <v>15</v>
       </c>
       <c r="J79" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
@@ -2262,22 +2274,22 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C80" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D80" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I80" t="s">
         <v>15</v>
       </c>
       <c r="J80" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
@@ -2285,19 +2297,19 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C81" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="H81" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I81" t="s">
         <v>15</v>
       </c>
       <c r="J81" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.35">
@@ -2305,22 +2317,22 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C82" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D82" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H82" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I82" t="s">
         <v>15</v>
       </c>
       <c r="J82" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
@@ -2350,13 +2362,13 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I85" t="s">
         <v>11</v>
       </c>
       <c r="J85" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
@@ -2364,13 +2376,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I86" t="s">
         <v>11</v>
       </c>
       <c r="J86" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
@@ -2378,13 +2390,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I87" t="s">
         <v>11</v>
       </c>
       <c r="J87" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.35">
@@ -2392,13 +2404,13 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I88" t="s">
         <v>11</v>
       </c>
       <c r="J88" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
@@ -2428,13 +2440,13 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I91" t="s">
         <v>11</v>
       </c>
       <c r="J91" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.35">
@@ -2442,13 +2454,13 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I92" t="s">
         <v>11</v>
       </c>
       <c r="J92" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.35">
@@ -2456,13 +2468,13 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="I93" t="s">
         <v>11</v>
       </c>
       <c r="J93" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.35">
@@ -2470,13 +2482,13 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I94" t="s">
         <v>11</v>
       </c>
       <c r="J94" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.35">
@@ -2506,13 +2518,13 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="I97" t="s">
         <v>11</v>
       </c>
       <c r="J97" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.35">
@@ -2520,13 +2532,13 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I98" t="s">
         <v>11</v>
       </c>
       <c r="J98" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.35">
@@ -2534,13 +2546,13 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I99" t="s">
         <v>11</v>
       </c>
       <c r="J99" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.35">
@@ -2548,13 +2560,13 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="I100" t="s">
         <v>11</v>
       </c>
       <c r="J100" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.35">
@@ -2587,9 +2599,9 @@
       <c r="I103" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:J2" xr:uid="{66DCD8A4-7681-4B36-987C-6CF98CBE9C65}">
+  <autoFilter ref="A2:J102" xr:uid="{66DCD8A4-7681-4B36-987C-6CF98CBE9C65}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J102">
-      <sortCondition ref="A2"/>
+      <sortCondition ref="A2:A102"/>
     </sortState>
   </autoFilter>
   <mergeCells count="1">

</xml_diff>

<commit_message>
add 1099EMB stuff, fixed SoM libs, updated readmes
</commit_message>
<xml_diff>
--- a/SoMs/BW1099/BW1099_IO_TABLE.xlsx
+++ b/SoMs/BW1099/BW1099_IO_TABLE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BrianLuxonis\Desktop\hardware\Luxonis_HW_Documentation\BW1099 Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B177EBB-F78F-435D-B03A-0E59207A5B35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E25EB8-747F-4678-871E-8F3FA4D189CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{2A677646-14BE-4F73-937F-BE4037A1016C}"/>
+    <workbookView xWindow="7180" yWindow="3170" windowWidth="24570" windowHeight="17130" xr2:uid="{2A677646-14BE-4F73-937F-BE4037A1016C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -999,10 +999,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A708E1D-7DB8-4706-8500-09B1FAE3DD99}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1062,7 +1063,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1073,7 +1074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1084,7 +1085,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1121,7 +1122,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1158,7 +1159,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1169,7 +1170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1180,7 +1181,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1194,7 +1195,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1208,7 +1209,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1222,7 +1223,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1236,7 +1237,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1247,7 +1248,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1258,7 +1259,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1272,7 +1273,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1286,7 +1287,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1300,7 +1301,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1314,7 +1315,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1325,7 +1326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1336,7 +1337,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1350,7 +1351,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1364,7 +1365,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1378,7 +1379,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1392,7 +1393,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1403,7 +1404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1414,7 +1415,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1448,7 +1449,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1462,7 +1463,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1473,7 +1474,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1484,30 +1485,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C34" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D34" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="E34" t="s">
-        <v>190</v>
+        <v>79</v>
       </c>
       <c r="F34" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="G34" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="H34" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="I34" t="s">
         <v>58</v>
@@ -1576,21 +1577,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="B38" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C38" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="D38" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="E38" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="H38" t="s">
         <v>69</v>
@@ -1602,7 +1603,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1619,24 +1620,24 @@
         <v>187</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C40" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="E40" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="G40" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="H40" t="s">
         <v>69</v>
@@ -1648,7 +1649,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1665,30 +1666,30 @@
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B42" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C42" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D42" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="E42" t="s">
-        <v>79</v>
+        <v>190</v>
       </c>
       <c r="F42" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="G42" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="H42" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="I42" t="s">
         <v>58</v>
@@ -1697,7 +1698,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1731,7 +1732,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1742,7 +1743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1753,7 +1754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1764,7 +1765,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1775,7 +1776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1789,7 +1790,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1803,7 +1804,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1817,7 +1818,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1831,7 +1832,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>51</v>
       </c>
@@ -1845,7 +1846,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>52</v>
       </c>
@@ -1859,7 +1860,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>53</v>
       </c>
@@ -1873,7 +1874,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>54</v>
       </c>
@@ -1887,7 +1888,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>55</v>
       </c>
@@ -1898,7 +1899,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>56</v>
       </c>
@@ -1909,7 +1910,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>57</v>
       </c>
@@ -1920,7 +1921,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>58</v>
       </c>
@@ -1971,21 +1972,21 @@
         <v>183</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B63" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C63" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D63" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E63" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="H63" t="s">
         <v>69</v>
@@ -2014,24 +2015,24 @@
         <v>182</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="B65" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C65" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D65" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E65" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="G65" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="H65" t="s">
         <v>69</v>
@@ -2168,7 +2169,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>71</v>
       </c>
@@ -2179,7 +2180,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>72</v>
       </c>
@@ -2227,7 +2228,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>75</v>
       </c>
@@ -2238,7 +2239,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>76</v>
       </c>
@@ -2335,7 +2336,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>81</v>
       </c>
@@ -2346,7 +2347,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>82</v>
       </c>
@@ -2357,7 +2358,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>83</v>
       </c>
@@ -2371,7 +2372,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>84</v>
       </c>
@@ -2385,7 +2386,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>85</v>
       </c>
@@ -2399,7 +2400,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>86</v>
       </c>
@@ -2413,7 +2414,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>87</v>
       </c>
@@ -2424,7 +2425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>88</v>
       </c>
@@ -2435,7 +2436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>89</v>
       </c>
@@ -2449,7 +2450,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>90</v>
       </c>
@@ -2463,7 +2464,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>91</v>
       </c>
@@ -2477,7 +2478,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>92</v>
       </c>
@@ -2491,7 +2492,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>93</v>
       </c>
@@ -2502,7 +2503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>94</v>
       </c>
@@ -2513,7 +2514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>95</v>
       </c>
@@ -2527,7 +2528,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>96</v>
       </c>
@@ -2541,7 +2542,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>97</v>
       </c>
@@ -2555,7 +2556,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>98</v>
       </c>
@@ -2569,7 +2570,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>99</v>
       </c>
@@ -2580,7 +2581,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>100</v>
       </c>
@@ -2600,7 +2601,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:J102" xr:uid="{66DCD8A4-7681-4B36-987C-6CF98CBE9C65}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J102">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="1.8V GPIO"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:J82">
       <sortCondition ref="A2:A102"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Updated doc revisions & add EMB/2099 corrections
</commit_message>
<xml_diff>
--- a/SoMs/BW1099/BW1099_IO_TABLE.xlsx
+++ b/SoMs/BW1099/BW1099_IO_TABLE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BrianLuxonis\Desktop\hardware\Luxonis_HW_Documentation\BW1099 Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E25EB8-747F-4678-871E-8F3FA4D189CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BABA71-B869-4C6D-9A8F-0D7460BDC99C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7180" yWindow="3170" windowWidth="24570" windowHeight="17130" xr2:uid="{2A677646-14BE-4F73-937F-BE4037A1016C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{2A677646-14BE-4F73-937F-BE4037A1016C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -999,11 +999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A708E1D-7DB8-4706-8500-09B1FAE3DD99}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D114" sqref="D114"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1063,7 +1062,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1074,7 +1073,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1085,7 +1084,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1122,7 +1121,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1159,7 +1158,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1170,7 +1169,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1181,7 +1180,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1195,7 +1194,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1209,7 +1208,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1223,7 +1222,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1237,7 +1236,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1248,7 +1247,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1259,7 +1258,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1273,7 +1272,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1287,7 +1286,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1301,7 +1300,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1315,7 +1314,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1326,7 +1325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1337,7 +1336,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1351,7 +1350,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1365,7 +1364,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1379,7 +1378,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1393,7 +1392,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1404,7 +1403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1415,7 +1414,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1449,7 +1448,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1463,7 +1462,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1474,7 +1473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1485,7 +1484,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>40</v>
       </c>
@@ -1577,7 +1576,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>61</v>
       </c>
@@ -1603,7 +1602,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1620,7 +1619,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>63</v>
       </c>
@@ -1649,7 +1648,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1666,7 +1665,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>32</v>
       </c>
@@ -1698,7 +1697,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1732,7 +1731,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1743,7 +1742,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1754,7 +1753,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1765,7 +1764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1776,7 +1775,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1790,7 +1789,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1804,7 +1803,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1818,7 +1817,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1832,7 +1831,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>51</v>
       </c>
@@ -1846,7 +1845,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>52</v>
       </c>
@@ -1860,7 +1859,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>53</v>
       </c>
@@ -1874,7 +1873,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>54</v>
       </c>
@@ -1888,7 +1887,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>55</v>
       </c>
@@ -1899,7 +1898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>56</v>
       </c>
@@ -1910,7 +1909,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>57</v>
       </c>
@@ -1921,7 +1920,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>58</v>
       </c>
@@ -1972,7 +1971,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>36</v>
       </c>
@@ -2015,7 +2014,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>38</v>
       </c>
@@ -2169,7 +2168,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>71</v>
       </c>
@@ -2180,7 +2179,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>72</v>
       </c>
@@ -2228,7 +2227,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>75</v>
       </c>
@@ -2239,7 +2238,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>76</v>
       </c>
@@ -2281,16 +2280,16 @@
         <v>163</v>
       </c>
       <c r="D80" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="H80" t="s">
         <v>61</v>
       </c>
-      <c r="I80" t="s">
+      <c r="I80" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J80" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
@@ -2306,7 +2305,7 @@
       <c r="H81" t="s">
         <v>61</v>
       </c>
-      <c r="I81" t="s">
+      <c r="I81" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J81" t="s">
@@ -2324,19 +2323,19 @@
         <v>165</v>
       </c>
       <c r="D82" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="H82" t="s">
         <v>61</v>
       </c>
-      <c r="I82" t="s">
+      <c r="I82" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J82" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>81</v>
       </c>
@@ -2347,7 +2346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>82</v>
       </c>
@@ -2358,7 +2357,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>83</v>
       </c>
@@ -2372,7 +2371,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>84</v>
       </c>
@@ -2386,7 +2385,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>85</v>
       </c>
@@ -2400,7 +2399,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>86</v>
       </c>
@@ -2414,7 +2413,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>87</v>
       </c>
@@ -2425,7 +2424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>88</v>
       </c>
@@ -2436,7 +2435,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>89</v>
       </c>
@@ -2450,7 +2449,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>90</v>
       </c>
@@ -2464,7 +2463,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>91</v>
       </c>
@@ -2478,7 +2477,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>92</v>
       </c>
@@ -2492,7 +2491,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>93</v>
       </c>
@@ -2503,7 +2502,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>94</v>
       </c>
@@ -2514,7 +2513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>95</v>
       </c>
@@ -2528,7 +2527,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>96</v>
       </c>
@@ -2542,7 +2541,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>97</v>
       </c>
@@ -2556,7 +2555,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>98</v>
       </c>
@@ -2570,7 +2569,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>99</v>
       </c>
@@ -2581,7 +2580,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>100</v>
       </c>
@@ -2600,16 +2599,6 @@
       <c r="I103" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:J102" xr:uid="{66DCD8A4-7681-4B36-987C-6CF98CBE9C65}">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="1.8V GPIO"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:J82">
-      <sortCondition ref="A2:A102"/>
-    </sortState>
-  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Updated connector GPIO pin names and related documentation
</commit_message>
<xml_diff>
--- a/SoMs/BW1099/BW1099_IO_TABLE.xlsx
+++ b/SoMs/BW1099/BW1099_IO_TABLE.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="198">
   <si>
     <t>Pin #</t>
   </si>
@@ -441,117 +441,9 @@
     <t>Camera C MIPI clock (+) / 0.5ps intra-pair tuning / 1ps inter-pair tuning / 100ohm +/-10%</t>
   </si>
   <si>
-    <t>SGPIO_1</t>
-  </si>
-  <si>
-    <t>SGPIO_2</t>
-  </si>
-  <si>
-    <t>SGPIO_3</t>
-  </si>
-  <si>
-    <t>SGPIO_4</t>
-  </si>
-  <si>
-    <t>SGPIO_5</t>
-  </si>
-  <si>
-    <t>SGPIO_6</t>
-  </si>
-  <si>
-    <t>SGPIO_7</t>
-  </si>
-  <si>
-    <t>SGPIO_8</t>
-  </si>
-  <si>
-    <t>SGPIO_9</t>
-  </si>
-  <si>
-    <t>SGPIO_10</t>
-  </si>
-  <si>
-    <t>SGPIO_11</t>
-  </si>
-  <si>
-    <t>SGPIO_12</t>
-  </si>
-  <si>
-    <t>SGPIO_13</t>
-  </si>
-  <si>
-    <t>SGPIO_14</t>
-  </si>
-  <si>
-    <t>SGPIO_15</t>
-  </si>
-  <si>
-    <t>SGPIO_16</t>
-  </si>
-  <si>
-    <t>SGPIO_17</t>
-  </si>
-  <si>
-    <t>SGPIO_18</t>
-  </si>
-  <si>
-    <t>SGPIO_19</t>
-  </si>
-  <si>
-    <t>SGPIO_20</t>
-  </si>
-  <si>
-    <t>SGPIO_21</t>
-  </si>
-  <si>
-    <t>SGPIO_22</t>
-  </si>
-  <si>
-    <t>SGPIO_23</t>
-  </si>
-  <si>
-    <t>SGPIO_24</t>
-  </si>
-  <si>
-    <t>SGPIO_25</t>
-  </si>
-  <si>
-    <t>SGPIO_26</t>
-  </si>
-  <si>
-    <t>SGPIO_27</t>
-  </si>
-  <si>
-    <t>SGPIO_28</t>
-  </si>
-  <si>
-    <t>SGPIO_29</t>
-  </si>
-  <si>
-    <t>SGPIO_4_3V3</t>
-  </si>
-  <si>
-    <t>SGPIO_8_3V3</t>
-  </si>
-  <si>
-    <t>SGPIO_9_3V3</t>
-  </si>
-  <si>
-    <t>SGPIO_10_3V3</t>
-  </si>
-  <si>
     <t>SPI0_CS_0</t>
   </si>
   <si>
-    <t>SGPIO_16_3V3</t>
-  </si>
-  <si>
-    <t>SGPIO_14_3V3</t>
-  </si>
-  <si>
-    <t>SGPIO_13/SPI0_CS_1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> SoM GPIO</t>
   </si>
   <si>
@@ -597,9 +489,6 @@
     <t xml:space="preserve">SoM system reset. Leave floating if unused. </t>
   </si>
   <si>
-    <t xml:space="preserve">Leave floating.  Any SGPIO pin can be used to wake up the SoM. </t>
-  </si>
-  <si>
     <t>spi2_cs_0</t>
   </si>
   <si>
@@ -610,6 +499,132 @@
   </si>
   <si>
     <t xml:space="preserve">Auxiliary GPIO for cameras sync/trigger. Reserved for interrupt FSIN (Frame sync input) for the cameras used. </t>
+  </si>
+  <si>
+    <t>GPIO_46</t>
+  </si>
+  <si>
+    <t>GPIO_45</t>
+  </si>
+  <si>
+    <t>GPIO_44</t>
+  </si>
+  <si>
+    <t>GPIO_34_3V3</t>
+  </si>
+  <si>
+    <t>GPIO_34</t>
+  </si>
+  <si>
+    <t>GPIO_21</t>
+  </si>
+  <si>
+    <t>GPIO_20</t>
+  </si>
+  <si>
+    <t>GPIO_31</t>
+  </si>
+  <si>
+    <t>GPIO_33_3V3</t>
+  </si>
+  <si>
+    <t>GPIO_32_3V3</t>
+  </si>
+  <si>
+    <t>GPIO_37_3V3</t>
+  </si>
+  <si>
+    <t>GPIO_36_3V3</t>
+  </si>
+  <si>
+    <t>GPIO_35_3V3</t>
+  </si>
+  <si>
+    <t>GPIO_41</t>
+  </si>
+  <si>
+    <t>GPIO_7_3V3</t>
+  </si>
+  <si>
+    <t>GPIO_7</t>
+  </si>
+  <si>
+    <t>GPIO_8/SPI0_CS_1</t>
+  </si>
+  <si>
+    <t>GPIO_8</t>
+  </si>
+  <si>
+    <t>GPIO_0</t>
+  </si>
+  <si>
+    <t>GPIO_1</t>
+  </si>
+  <si>
+    <t>GPIO_2</t>
+  </si>
+  <si>
+    <t>GPIO_3</t>
+  </si>
+  <si>
+    <t>GPIO_57</t>
+  </si>
+  <si>
+    <t>GPIO_54</t>
+  </si>
+  <si>
+    <t>GPIO_53</t>
+  </si>
+  <si>
+    <t>GPIO_5</t>
+  </si>
+  <si>
+    <t>GPIO_47</t>
+  </si>
+  <si>
+    <t>GPIO_4</t>
+  </si>
+  <si>
+    <t>GPIO_22</t>
+  </si>
+  <si>
+    <t>GPIO_23</t>
+  </si>
+  <si>
+    <t>I2C2_SCL</t>
+  </si>
+  <si>
+    <t>I2C2_SDA</t>
+  </si>
+  <si>
+    <t>I2C1_SCL</t>
+  </si>
+  <si>
+    <t>I2C1_SDA</t>
+  </si>
+  <si>
+    <t>GPIO_24</t>
+  </si>
+  <si>
+    <t>GPIO_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leave floating.  Any GPIO pin can be used to wake up the SoM. </t>
+  </si>
+  <si>
+    <t>GPIO_37</t>
+  </si>
+  <si>
+    <t>GPIO_36</t>
+  </si>
+  <si>
+    <t>GPIO_35</t>
+  </si>
+  <si>
+    <t>GPIO_32</t>
+  </si>
+  <si>
+    <t>GPIO_33</t>
   </si>
 </sst>
 </file>
@@ -985,7 +1000,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -995,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,7 +1027,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>175</v>
+        <v>139</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1032,7 +1047,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>173</v>
+        <v>137</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
@@ -1053,7 +1068,7 @@
         <v>7</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>185</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1097,10 +1112,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="C6" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -1112,7 +1127,7 @@
         <v>15</v>
       </c>
       <c r="J6" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1134,10 +1149,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="C8" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
@@ -1149,7 +1164,7 @@
         <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1430,7 +1445,7 @@
         <v>49</v>
       </c>
       <c r="C30" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="H30" t="s">
         <v>50</v>
@@ -1480,34 +1495,34 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C34" t="s">
-        <v>145</v>
+        <v>193</v>
       </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="E34" t="s">
-        <v>79</v>
+        <v>152</v>
       </c>
       <c r="F34" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="G34" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="H34" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="I34" t="s">
         <v>58</v>
       </c>
       <c r="J34" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1518,9 +1533,12 @@
         <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="D35" t="s">
+        <v>189</v>
+      </c>
+      <c r="E35" t="s">
         <v>60</v>
       </c>
       <c r="H35" t="s">
@@ -1541,7 +1559,7 @@
         <v>63</v>
       </c>
       <c r="C36" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="I36" t="s">
         <v>15</v>
@@ -1558,7 +1576,10 @@
         <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>142</v>
+        <v>162</v>
+      </c>
+      <c r="D37" t="s">
+        <v>188</v>
       </c>
       <c r="H37" t="s">
         <v>61</v>
@@ -1572,19 +1593,19 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C38" t="s">
-        <v>149</v>
+        <v>194</v>
       </c>
       <c r="D38" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="E38" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="H38" t="s">
         <v>69</v>
@@ -1593,7 +1614,7 @@
         <v>58</v>
       </c>
       <c r="J38" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -1610,27 +1631,27 @@
         <v>72</v>
       </c>
       <c r="J39" t="s">
-        <v>186</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C40" t="s">
-        <v>151</v>
+        <v>195</v>
       </c>
       <c r="D40" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="E40" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="G40" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="H40" t="s">
         <v>69</v>
@@ -1639,7 +1660,7 @@
         <v>58</v>
       </c>
       <c r="J40" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -1656,39 +1677,39 @@
         <v>77</v>
       </c>
       <c r="J41" t="s">
-        <v>187</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C42" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="D42" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="E42" t="s">
-        <v>189</v>
+        <v>79</v>
       </c>
       <c r="F42" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="G42" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="H42" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="I42" t="s">
         <v>58</v>
       </c>
       <c r="J42" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -1705,7 +1726,7 @@
         <v>77</v>
       </c>
       <c r="J43" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -1716,13 +1737,13 @@
         <v>84</v>
       </c>
       <c r="C44" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="I44" t="s">
         <v>15</v>
       </c>
       <c r="J44" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -1930,10 +1951,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="C61" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="H61" t="s">
         <v>69</v>
@@ -1942,7 +1963,7 @@
         <v>15</v>
       </c>
       <c r="J61" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -1953,7 +1974,7 @@
         <v>172</v>
       </c>
       <c r="C62" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="D62" t="s">
         <v>89</v>
@@ -1962,24 +1983,24 @@
         <v>15</v>
       </c>
       <c r="J62" t="s">
-        <v>182</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C63" t="s">
-        <v>143</v>
+        <v>196</v>
       </c>
       <c r="D63" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="E63" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="H63" t="s">
         <v>69</v>
@@ -1988,7 +2009,7 @@
         <v>58</v>
       </c>
       <c r="J63" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -1999,33 +2020,33 @@
         <v>92</v>
       </c>
       <c r="C64" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="I64" t="s">
         <v>15</v>
       </c>
       <c r="J64" t="s">
-        <v>181</v>
+        <v>145</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C65" t="s">
-        <v>144</v>
+        <v>197</v>
       </c>
       <c r="D65" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="E65" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="G65" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="H65" t="s">
         <v>69</v>
@@ -2034,7 +2055,7 @@
         <v>58</v>
       </c>
       <c r="J65" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
@@ -2045,13 +2066,13 @@
         <v>96</v>
       </c>
       <c r="C66" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
       <c r="I66" t="s">
         <v>15</v>
       </c>
       <c r="J66" t="s">
-        <v>180</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -2062,7 +2083,7 @@
         <v>97</v>
       </c>
       <c r="C67" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="I67" t="s">
         <v>15</v>
@@ -2079,7 +2100,7 @@
         <v>99</v>
       </c>
       <c r="C68" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="H68" t="s">
         <v>102</v>
@@ -2088,7 +2109,7 @@
         <v>15</v>
       </c>
       <c r="J68" t="s">
-        <v>179</v>
+        <v>143</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -2096,10 +2117,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>174</v>
+        <v>138</v>
       </c>
       <c r="C69" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="I69" t="s">
         <v>15</v>
@@ -2116,7 +2137,7 @@
         <v>101</v>
       </c>
       <c r="C70" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="H70" t="s">
         <v>102</v>
@@ -2125,7 +2146,7 @@
         <v>15</v>
       </c>
       <c r="J70" t="s">
-        <v>178</v>
+        <v>142</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
@@ -2133,10 +2154,10 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="C71" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="I71" t="s">
         <v>15</v>
@@ -2147,10 +2168,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="C72" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="H72" t="s">
         <v>102</v>
@@ -2159,7 +2180,7 @@
         <v>15</v>
       </c>
       <c r="J72" t="s">
-        <v>177</v>
+        <v>141</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
@@ -2192,7 +2213,7 @@
         <v>103</v>
       </c>
       <c r="C75" t="s">
-        <v>159</v>
+        <v>182</v>
       </c>
       <c r="H75" t="s">
         <v>50</v>
@@ -2212,13 +2233,13 @@
         <v>105</v>
       </c>
       <c r="C76" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="I76" t="s">
         <v>15</v>
       </c>
       <c r="J76" t="s">
-        <v>176</v>
+        <v>140</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
@@ -2251,7 +2272,10 @@
         <v>106</v>
       </c>
       <c r="C79" t="s">
-        <v>161</v>
+        <v>184</v>
+      </c>
+      <c r="D79" t="s">
+        <v>186</v>
       </c>
       <c r="H79" t="s">
         <v>61</v>
@@ -2268,10 +2292,10 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="C80" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="D80" t="s">
         <v>95</v>
@@ -2294,7 +2318,10 @@
         <v>109</v>
       </c>
       <c r="C81" t="s">
-        <v>163</v>
+        <v>185</v>
+      </c>
+      <c r="D81" t="s">
+        <v>187</v>
       </c>
       <c r="H81" t="s">
         <v>61</v>
@@ -2311,10 +2338,10 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>164</v>
+        <v>191</v>
       </c>
       <c r="C82" t="s">
-        <v>164</v>
+        <v>191</v>
       </c>
       <c r="D82" t="s">
         <v>81</v>
@@ -2593,6 +2620,11 @@
       <c r="I103" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:J102">
+    <sortState ref="A6:J82">
+      <sortCondition ref="A2:A102"/>
+    </sortState>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>

</xml_diff>